<commit_message>
Integrated the new CLNE model run into the graphs and debugged some protease substrate relationship issues.
</commit_message>
<xml_diff>
--- a/models/ecoli/analysis/local_notebooks/C_limited_PDR_analyses_with_published_paper_data/supplementary_data/ST2_prioritysort2_substrates.xlsx
+++ b/models/ecoli/analysis/local_notebooks/C_limited_PDR_analyses_with_published_paper_data/supplementary_data/ST2_prioritysort2_substrates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/miagrahn/wcEcoli/models/ecoli/analysis/local_notebooks/C_limited_PDR_analyses_with_published_paper_data/supplementary_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59EF854C-018C-AA4C-A9E3-1EAD42FBEB7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0CB5DCC-CA4C-8F4A-9A4C-968F64F86B0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2720" yWindow="3600" windowWidth="27640" windowHeight="16940" xr2:uid="{8EBBFE47-E0CD-C74B-986A-696C3F792D5E}"/>
   </bookViews>
@@ -485,9 +485,6 @@
     <t>sp|P76340|YEDW_ECOLI</t>
   </si>
   <si>
-    <t>yedW</t>
-  </si>
-  <si>
     <t>sp|P0ADK6|YIBA_ECOLI</t>
   </si>
   <si>
@@ -521,9 +518,6 @@
     <t>sp|P37338|CSIR_ECOLI</t>
   </si>
   <si>
-    <t>csiR</t>
-  </si>
-  <si>
     <t>sp|P21507|SRMB_ECOLI</t>
   </si>
   <si>
@@ -564,6 +558,12 @@
   </si>
   <si>
     <t>yiaU</t>
+  </si>
+  <si>
+    <t>hprR</t>
+  </si>
+  <si>
+    <t>glaR</t>
   </si>
 </sst>
 </file>
@@ -1064,8 +1064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98D4331D-9240-454D-A4AB-921DE3B5E341}">
   <dimension ref="A1:H92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="K78" sqref="K78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2869,7 +2869,7 @@
         <v>148</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>149</v>
+        <v>174</v>
       </c>
       <c r="C70" s="5" t="s">
         <v>107</v>
@@ -2892,10 +2892,10 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="B71" s="5" t="s">
         <v>150</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>151</v>
       </c>
       <c r="C71" s="5" t="s">
         <v>107</v>
@@ -2918,10 +2918,10 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B72" s="5" t="s">
         <v>152</v>
-      </c>
-      <c r="B72" s="5" t="s">
-        <v>153</v>
       </c>
       <c r="C72" s="5" t="s">
         <v>107</v>
@@ -2944,10 +2944,10 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="B73" s="5" t="s">
         <v>154</v>
-      </c>
-      <c r="B73" s="5" t="s">
-        <v>155</v>
       </c>
       <c r="C73" s="5" t="s">
         <v>107</v>
@@ -2970,10 +2970,10 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="B74" s="5" t="s">
         <v>156</v>
-      </c>
-      <c r="B74" s="5" t="s">
-        <v>157</v>
       </c>
       <c r="C74" s="5" t="s">
         <v>107</v>
@@ -2996,10 +2996,10 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="B75" s="5" t="s">
         <v>158</v>
-      </c>
-      <c r="B75" s="5" t="s">
-        <v>159</v>
       </c>
       <c r="C75" s="5" t="s">
         <v>107</v>
@@ -3022,10 +3022,10 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>161</v>
+        <v>175</v>
       </c>
       <c r="C76" s="5" t="s">
         <v>107</v>
@@ -3048,10 +3048,10 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C77" s="5" t="s">
         <v>107</v>
@@ -3074,10 +3074,10 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C78" s="5" t="s">
         <v>107</v>
@@ -3100,10 +3100,10 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C79" s="5" t="s">
         <v>107</v>
@@ -3126,10 +3126,10 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C80" s="5" t="s">
         <v>107</v>
@@ -3152,10 +3152,10 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C81" s="5" t="s">
         <v>107</v>
@@ -3178,10 +3178,10 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C82" s="5" t="s">
         <v>107</v>
@@ -3204,10 +3204,10 @@
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C83" s="5" t="s">
         <v>107</v>

</xml_diff>